<commit_message>
Partial refactor of ETL code
</commit_message>
<xml_diff>
--- a/application/tests/import/test_new_data.xlsx
+++ b/application/tests/import/test_new_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/umpire/application/tests/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F376407-BE52-E64D-9BC2-D57A33C2C38A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017FEE59-4B2D-1C4F-8930-B1A75A04E4D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <t>David House</t>
   </si>
   <si>
-    <t>Lorne NEW TEAM</t>
-  </si>
-  <si>
     <t>AFL Barwon - 2018 Some New Competition</t>
   </si>
   <si>
@@ -197,6 +194,9 @@
   </si>
   <si>
     <t>Some new club</t>
+  </si>
+  <si>
+    <t>Lorne NEW TEAM 2</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A5"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,7 +740,7 @@
         <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
         <v>20</v>
@@ -834,7 +834,7 @@
         <v>43190</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
@@ -887,7 +887,7 @@
         <v>43190</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
@@ -899,7 +899,7 @@
         <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>46</v>

</xml_diff>